<commit_message>
Enclosure Finder Web API & SPA
</commit_message>
<xml_diff>
--- a/Refs/AltechEnclosureFinder.xlsx
+++ b/Refs/AltechEnclosureFinder.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="44200" windowHeight="17980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
-  <si>
-    <t>Type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Part Number</t>
   </si>
@@ -75,9 +72,6 @@
     <t>Depth (in)</t>
   </si>
   <si>
-    <t>IP Protection</t>
-  </si>
-  <si>
     <t>NEMA 4X</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>PC55-4-o</t>
   </si>
   <si>
-    <t>Enclosure 50x52x35mm, Polycarbonate, Gray, Smooth Sides</t>
-  </si>
-  <si>
     <t>Drawing</t>
   </si>
   <si>
@@ -103,6 +94,177 @@
   </si>
   <si>
     <t>UL approval</t>
+  </si>
+  <si>
+    <t>Polystyrene</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/PDFS/Splits/IndEnclo-20.pdf</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/EnclosureDwgs/TK/TK1111.DWG</t>
+  </si>
+  <si>
+    <t>105-404</t>
+  </si>
+  <si>
+    <t>PS1111-7-m</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/STEP-FILES/TK1111/105-404_and_127-404.stp</t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t>IP67</t>
+  </si>
+  <si>
+    <t>TGABS2012-8-to</t>
+  </si>
+  <si>
+    <t>101-008-01</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/PDFS/Splits/IndEnclo-57.pdf</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/EnclosureDwgs/TG/TG2012-8.dwg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/STEP-FILES/TG_StepFiles/TG2012-8/10100801.stp</t>
+  </si>
+  <si>
+    <t>TGPC3023-11-to</t>
+  </si>
+  <si>
+    <t>201-513-01</t>
+  </si>
+  <si>
+    <t>Enclosure, Polycarbonate, Gray, Smooth Sides</t>
+  </si>
+  <si>
+    <t>Enclosure, Polystyrene, Gray, Metric knockouts</t>
+  </si>
+  <si>
+    <t>Enclosure, Polycarbonate, Gray with transparent cover, smooth walls</t>
+  </si>
+  <si>
+    <t>Enclosure, ABS, Gray with transparent cover, quick turn screws, smooth walls</t>
+  </si>
+  <si>
+    <t>Enclosure, Polycarbonate, Gray with transparent cover, quick turn screws, smooth walls</t>
+  </si>
+  <si>
+    <t>201-513-91</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/PDFS/Splits/IndEnclo-63.pdf</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/EnclosureDwgs/TG/TG3023-11.dwg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/STEP-FILES/TG_StepFiles/TG3023-11/20151301.stp</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>AL1212-8</t>
+  </si>
+  <si>
+    <t>150-009</t>
+  </si>
+  <si>
+    <t>Enclosure, Cast Aluminum, Dark Gray</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/PDFS/Splits/IndEnclo-76.pdf</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/EnclosureDwgs/AL/AL1212-8.dwg</t>
+  </si>
+  <si>
+    <t>IP65</t>
+  </si>
+  <si>
+    <t>EK</t>
+  </si>
+  <si>
+    <t>EK004</t>
+  </si>
+  <si>
+    <t>542-504</t>
+  </si>
+  <si>
+    <t>Enclosure with access door for up to 4 poles DIN Circuit breakers, Polycarbonate, Gray, smooth walls</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/PDFS/Splits/IndEnclo-117.pdf</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/EnclosureDwgs/EK/EK004.dwg</t>
+  </si>
+  <si>
+    <t>PC1811-11-o</t>
+  </si>
+  <si>
+    <t>120-906</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/PDFS/Splits/IndEnclo-30.pdf</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/EnclosureDwgs/TK/TK1811.DWG</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/enclosures/STEP-FILES/TK1811/110-906_and_120-906.stp</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/ImageBank/Enclosures/101008.jpg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/ImageBank/Enclosures/105404.jpg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/ImageBank/Enclosures/20151301.jpg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/ImageBank/Enclosures/20151391.jpg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/ImageBank/Enclosures/150009.jpg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/ImageBank/Enclosures/542504.jpg</t>
+  </si>
+  <si>
+    <t>http://www.altechcorp.com/ImageBank/Enclosures/120906.jpg</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Ingress  Protection</t>
+  </si>
+  <si>
+    <t>Type Number</t>
   </si>
 </sst>
 </file>
@@ -141,18 +303,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,21 +325,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -522,142 +675,563 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14" style="2" customWidth="1"/>
-    <col min="9" max="10" width="12.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11" style="2"/>
-    <col min="13" max="13" width="13.25" style="2" customWidth="1"/>
-    <col min="14" max="14" width="50.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="49.25" style="2" customWidth="1"/>
-    <col min="16" max="16" width="51.125" style="2" customWidth="1"/>
-    <col min="17" max="18" width="58.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.83203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="84.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="61.33203125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="51.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="63.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="76.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3">
+        <v>1.77</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.38</v>
+      </c>
+      <c r="D2" s="3">
+        <v>45</v>
+      </c>
+      <c r="E2" s="3">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3">
+        <v>35</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>110</v>
+      </c>
+      <c r="E3" s="3">
+        <v>110</v>
+      </c>
+      <c r="F3" s="3">
+        <v>66</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>25</v>
+      <c r="R3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1.77</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1.38</v>
-      </c>
-      <c r="D2" s="2">
+    <row r="4" spans="1:19">
+      <c r="A4" s="3">
+        <v>7.95</v>
+      </c>
+      <c r="B4" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.95</v>
+      </c>
+      <c r="D4" s="3">
+        <v>202</v>
+      </c>
+      <c r="E4" s="3">
+        <v>122</v>
+      </c>
+      <c r="F4" s="3">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="3">
+        <v>11.89</v>
+      </c>
+      <c r="B5" s="3">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="D5" s="3">
+        <v>302</v>
+      </c>
+      <c r="E5" s="3">
+        <v>232</v>
+      </c>
+      <c r="F5" s="3">
+        <v>110</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="2">
+      <c r="P5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="3">
+        <v>11.89</v>
+      </c>
+      <c r="B6" s="3">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="D6" s="3">
+        <v>302</v>
+      </c>
+      <c r="E6" s="3">
+        <v>232</v>
+      </c>
+      <c r="F6" s="3">
+        <v>110</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="2">
-        <v>35</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="4" t="s">
+      <c r="M6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4.72</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.15</v>
+      </c>
+      <c r="D7" s="3">
+        <v>122</v>
+      </c>
+      <c r="E7" s="3">
+        <v>120</v>
+      </c>
+      <c r="F7" s="3">
+        <v>80</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="4" t="s">
+      <c r="I7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="3">
+        <v>7.09</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="D8" s="3">
+        <v>180</v>
+      </c>
+      <c r="E8" s="3">
+        <v>110</v>
+      </c>
+      <c r="F8" s="3">
+        <v>110</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>24</v>
+      <c r="H8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="3">
+        <v>7.09</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4.33</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.37</v>
+      </c>
+      <c r="D9" s="3">
+        <v>180</v>
+      </c>
+      <c r="E9" s="3">
+        <v>110</v>
+      </c>
+      <c r="F9" s="3">
+        <v>111</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>